<commit_message>
Corretto bug nell'inserimento dell'azienda
</commit_message>
<xml_diff>
--- a/pages/super_user/inserimento/aziende/Stage_Manager_Modulo_Aziende.xlsx
+++ b/pages/super_user/inserimento/aziende/Stage_Manager_Modulo_Aziende.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -152,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -178,11 +178,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,9 +200,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -545,7 +548,7 @@
   <dimension ref="A1:AU1165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
     <col min="2" max="2" width="31.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="13" customWidth="1"/>
     <col min="6" max="10" width="29.5703125" style="5" customWidth="1"/>
     <col min="11" max="11" width="29.5703125" style="4" customWidth="1"/>
     <col min="12" max="35" width="18.28515625" style="1" customWidth="1"/>
@@ -574,7 +577,7 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -597,592 +600,592 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15"/>
+      <c r="A3" s="9"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15"/>
-      <c r="M4" s="13" t="s">
+      <c r="A4" s="9"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
+      <c r="M4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
+      <c r="A5" s="9"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="9"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="15"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="A6" s="9"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="9"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="15"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="A7" s="9"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="9"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
     </row>
     <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="15"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
+      <c r="A8" s="9"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="9"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
     </row>
     <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="15"/>
+      <c r="A9" s="9"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="15"/>
-      <c r="M10" s="14" t="s">
+      <c r="A10" s="9"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="9"/>
+      <c r="M10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="15"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
+      <c r="A11" s="9"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="9"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="15"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
+      <c r="A12" s="9"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="9"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
     </row>
     <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="15"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
+      <c r="A13" s="9"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="9"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="15"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
+      <c r="A14" s="9"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="9"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
     </row>
     <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="9"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="A16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="9"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="9"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="9"/>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="9"/>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="9"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="F25" s="12"/>
+      <c r="A25" s="9"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="F26" s="12"/>
+      <c r="A26" s="9"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="F27" s="12"/>
+      <c r="A27" s="9"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="F28" s="12"/>
+      <c r="A28" s="9"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="F29" s="12"/>
+      <c r="A29" s="9"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="F30" s="12"/>
+      <c r="A30" s="9"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="9"/>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="E32" s="10"/>
+      <c r="A32" s="9"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="E33" s="10"/>
+      <c r="A33" s="9"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="E34" s="10"/>
+      <c r="A34" s="9"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="E35" s="10"/>
+      <c r="A35" s="9"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="F36" s="12"/>
+      <c r="A36" s="9"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="F37" s="12"/>
+      <c r="A37" s="9"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="F38" s="12"/>
+      <c r="A38" s="9"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="F39" s="12"/>
+      <c r="A39" s="9"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="F40" s="12"/>
+      <c r="A40" s="9"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="F41" s="12"/>
+      <c r="A41" s="9"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="F42" s="12"/>
+      <c r="A42" s="9"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="F43" s="12"/>
+      <c r="A43" s="9"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
+      <c r="A44" s="9"/>
     </row>
     <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
+      <c r="A45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+      <c r="A46" s="9"/>
     </row>
     <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+      <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+      <c r="A48" s="9"/>
     </row>
     <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+      <c r="A49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+      <c r="A50" s="9"/>
     </row>
     <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+      <c r="A51" s="9"/>
     </row>
     <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="9"/>
     </row>
     <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="A53" s="9"/>
     </row>
     <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="9"/>
     </row>
     <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="E55" s="10"/>
+      <c r="A55" s="9"/>
+      <c r="E55" s="11"/>
     </row>
     <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="E56" s="10"/>
+      <c r="A56" s="9"/>
+      <c r="E56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="E57" s="10"/>
+      <c r="A57" s="9"/>
+      <c r="E57" s="11"/>
     </row>
     <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="E58" s="10"/>
+      <c r="A58" s="9"/>
+      <c r="E58" s="11"/>
     </row>
     <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+      <c r="A60" s="9"/>
     </row>
     <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="F61" s="12"/>
+      <c r="A61" s="9"/>
+      <c r="F61" s="14"/>
     </row>
     <row r="62" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="F62" s="12"/>
+      <c r="A62" s="9"/>
+      <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="F63" s="12"/>
+      <c r="A63" s="9"/>
+      <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="F64" s="12"/>
+      <c r="A64" s="9"/>
+      <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="F65" s="12"/>
+      <c r="A65" s="9"/>
+      <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
+      <c r="A66" s="9"/>
     </row>
     <row r="67" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="E67" s="10"/>
+      <c r="A67" s="9"/>
+      <c r="E67" s="11"/>
     </row>
     <row r="68" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="E68" s="10"/>
+      <c r="A68" s="9"/>
+      <c r="E68" s="11"/>
     </row>
     <row r="69" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="E69" s="10"/>
+      <c r="A69" s="9"/>
+      <c r="E69" s="11"/>
     </row>
     <row r="70" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="E70" s="10"/>
+      <c r="A70" s="9"/>
+      <c r="E70" s="11"/>
     </row>
     <row r="71" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
+      <c r="A71" s="9"/>
     </row>
     <row r="72" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+      <c r="A72" s="9"/>
     </row>
     <row r="73" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
+      <c r="A73" s="9"/>
     </row>
     <row r="74" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="F74" s="12"/>
+      <c r="A74" s="9"/>
+      <c r="F74" s="14"/>
     </row>
     <row r="75" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="F75" s="12"/>
+      <c r="A75" s="9"/>
+      <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="F76" s="12"/>
+      <c r="A76" s="9"/>
+      <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="F77" s="12"/>
+      <c r="A77" s="9"/>
+      <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="F78" s="12"/>
+      <c r="A78" s="9"/>
+      <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="F79" s="12"/>
+      <c r="A79" s="9"/>
+      <c r="F79" s="14"/>
     </row>
     <row r="80" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="F80" s="12"/>
+      <c r="A80" s="9"/>
+      <c r="F80" s="14"/>
     </row>
     <row r="81" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
-      <c r="F81" s="12"/>
+      <c r="A81" s="9"/>
+      <c r="F81" s="14"/>
     </row>
     <row r="82" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15"/>
+      <c r="A82" s="9"/>
     </row>
     <row r="83" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
+      <c r="A83" s="9"/>
     </row>
     <row r="84" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
+      <c r="A84" s="9"/>
     </row>
     <row r="85" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
+      <c r="A85" s="9"/>
     </row>
     <row r="86" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
+      <c r="A86" s="9"/>
     </row>
     <row r="87" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
+      <c r="A87" s="9"/>
     </row>
     <row r="88" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="E88" s="10"/>
+      <c r="A88" s="9"/>
+      <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
-      <c r="E89" s="10"/>
+      <c r="A89" s="9"/>
+      <c r="E89" s="11"/>
     </row>
     <row r="90" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="15"/>
-      <c r="E90" s="10"/>
+      <c r="A90" s="9"/>
+      <c r="E90" s="11"/>
     </row>
     <row r="91" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-      <c r="E91" s="10"/>
+      <c r="A91" s="9"/>
+      <c r="E91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15"/>
+      <c r="A92" s="9"/>
     </row>
     <row r="93" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-      <c r="F93" s="12"/>
+      <c r="A93" s="9"/>
+      <c r="F93" s="14"/>
     </row>
     <row r="94" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
-      <c r="F94" s="12"/>
+      <c r="A94" s="9"/>
+      <c r="F94" s="14"/>
     </row>
     <row r="95" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
-      <c r="F95" s="12"/>
+      <c r="A95" s="9"/>
+      <c r="F95" s="14"/>
     </row>
     <row r="96" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="15"/>
-      <c r="F96" s="12"/>
+      <c r="A96" s="9"/>
+      <c r="F96" s="14"/>
     </row>
     <row r="97" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-      <c r="F97" s="12"/>
+      <c r="A97" s="9"/>
+      <c r="F97" s="14"/>
     </row>
     <row r="98" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-      <c r="F98" s="12"/>
+      <c r="A98" s="9"/>
+      <c r="F98" s="14"/>
     </row>
     <row r="99" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="15"/>
+      <c r="A99" s="9"/>
     </row>
     <row r="100" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="15"/>
-      <c r="E100" s="10"/>
+      <c r="A100" s="9"/>
+      <c r="E100" s="11"/>
     </row>
     <row r="101" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="15"/>
-      <c r="E101" s="10"/>
+      <c r="A101" s="9"/>
+      <c r="E101" s="11"/>
     </row>
     <row r="102" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="15"/>
-      <c r="E102" s="10"/>
+      <c r="A102" s="9"/>
+      <c r="E102" s="11"/>
     </row>
     <row r="103" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="15"/>
-      <c r="E103" s="10"/>
+      <c r="A103" s="9"/>
+      <c r="E103" s="11"/>
     </row>
     <row r="104" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="15"/>
+      <c r="A104" s="9"/>
     </row>
     <row r="105" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
+      <c r="A105" s="9"/>
     </row>
     <row r="106" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="15"/>
+      <c r="A106" s="9"/>
     </row>
     <row r="107" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="15"/>
-      <c r="F107" s="12"/>
+      <c r="A107" s="9"/>
+      <c r="F107" s="14"/>
     </row>
     <row r="108" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
-      <c r="F108" s="12"/>
+      <c r="A108" s="9"/>
+      <c r="F108" s="14"/>
     </row>
     <row r="109" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="15"/>
-      <c r="F109" s="12"/>
+      <c r="A109" s="9"/>
+      <c r="F109" s="14"/>
     </row>
     <row r="110" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="15"/>
-      <c r="F110" s="12"/>
+      <c r="A110" s="9"/>
+      <c r="F110" s="14"/>
     </row>
     <row r="111" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="15"/>
-      <c r="F111" s="12"/>
+      <c r="A111" s="9"/>
+      <c r="F111" s="14"/>
     </row>
     <row r="112" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
-      <c r="F112" s="12"/>
+      <c r="A112" s="9"/>
+      <c r="F112" s="14"/>
     </row>
     <row r="113" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="15"/>
-      <c r="F113" s="12"/>
+      <c r="A113" s="9"/>
+      <c r="F113" s="14"/>
     </row>
     <row r="114" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="15"/>
-      <c r="F114" s="12"/>
+      <c r="A114" s="9"/>
+      <c r="F114" s="14"/>
     </row>
     <row r="115" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="15"/>
+      <c r="A115" s="9"/>
     </row>
     <row r="116" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
+      <c r="A116" s="9"/>
     </row>
     <row r="117" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="15"/>
-      <c r="E117" s="10"/>
+      <c r="A117" s="9"/>
+      <c r="E117" s="11"/>
     </row>
     <row r="118" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="15"/>
-      <c r="E118" s="10"/>
+      <c r="A118" s="9"/>
+      <c r="E118" s="11"/>
     </row>
     <row r="119" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="15"/>
-      <c r="E119" s="10"/>
+      <c r="A119" s="9"/>
+      <c r="E119" s="11"/>
     </row>
     <row r="120" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="15"/>
-      <c r="E120" s="10"/>
+      <c r="A120" s="9"/>
+      <c r="E120" s="11"/>
     </row>
     <row r="121" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="15"/>
+      <c r="A121" s="9"/>
     </row>
     <row r="122" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="15"/>
+      <c r="A122" s="9"/>
     </row>
     <row r="123" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="15"/>
-      <c r="F123" s="12"/>
+      <c r="A123" s="9"/>
+      <c r="F123" s="14"/>
     </row>
     <row r="124" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="15"/>
-      <c r="F124" s="12"/>
+      <c r="A124" s="9"/>
+      <c r="F124" s="14"/>
     </row>
     <row r="125" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="15"/>
-      <c r="F125" s="12"/>
+      <c r="A125" s="9"/>
+      <c r="F125" s="14"/>
     </row>
     <row r="126" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="15"/>
-      <c r="F126" s="12"/>
+      <c r="A126" s="9"/>
+      <c r="F126" s="14"/>
     </row>
     <row r="127" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="15"/>
-      <c r="F127" s="12"/>
+      <c r="A127" s="9"/>
+      <c r="F127" s="14"/>
     </row>
     <row r="128" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="15"/>
-      <c r="F128" s="12"/>
+      <c r="A128" s="9"/>
+      <c r="F128" s="14"/>
     </row>
     <row r="129" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="15"/>
-      <c r="F129" s="12"/>
+      <c r="A129" s="9"/>
+      <c r="F129" s="14"/>
     </row>
     <row r="130" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="15"/>
-      <c r="F130" s="12"/>
+      <c r="A130" s="9"/>
+      <c r="F130" s="14"/>
     </row>
     <row r="131" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="15"/>
-      <c r="F131" s="12"/>
+      <c r="A131" s="9"/>
+      <c r="F131" s="14"/>
     </row>
     <row r="132" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="15"/>
+      <c r="A132" s="9"/>
     </row>
     <row r="133" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="15"/>
+      <c r="A133" s="9"/>
     </row>
     <row r="134" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="15"/>
+      <c r="A134" s="9"/>
     </row>
     <row r="135" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="15"/>
+      <c r="A135" s="9"/>
     </row>
     <row r="136" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="15"/>
+      <c r="A136" s="9"/>
     </row>
     <row r="137" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="15"/>
+      <c r="A137" s="9"/>
     </row>
     <row r="138" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="139" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>